<commit_message>
Minor update to XLSX
</commit_message>
<xml_diff>
--- a/stat_tests/oa_target_data.xlsx
+++ b/stat_tests/oa_target_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yasminebassil/Documents/Emory/3_Research/Projects/NavAging_Paper/stat_tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{9FA66F95-5F79-4940-B779-248CFFDD26F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{9F7EA50B-538A-2B43-A0E1-E84B106F060C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1284,11 +1284,11 @@
   <dxfs count="6">
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1304,11 +1304,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1655,7 +1655,7 @@
   <dimension ref="A1:I197"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7584,14 +7584,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0.001</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
       <formula>0.01</formula>
       <formula>0.001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="between">
       <formula>0.05</formula>
       <formula>0.01</formula>
     </cfRule>

</xml_diff>